<commit_message>
Corrected blocks.xlsx data. Updated to 2022
</commit_message>
<xml_diff>
--- a/input/blocks.xlsx
+++ b/input/blocks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\Documents\09_Job\HiWi\02_Projekte\jupyter\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\Documents\09_Job\HiWi\02_Projekte\smard-data-processing\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCFB17B-4434-49D2-B6F7-F27DC67B26D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FF80CD-9866-4A0C-872B-DF3B99483512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1740" windowWidth="19440" windowHeight="10440" xr2:uid="{B3864E39-C3D2-F749-9175-08B59E08C58D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3864E39-C3D2-F749-9175-08B59E08C58D}"/>
   </bookViews>
   <sheets>
     <sheet name="Power plant blocks" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="660">
   <si>
     <t>Bexbach</t>
   </si>
@@ -1738,9 +1738,6 @@
     <t>Generation_DE Bexbach [MW]</t>
   </si>
   <si>
-    <t>Generation_DE GUD C 200</t>
-  </si>
-  <si>
     <t>Generation_DE Block 6 [MW]</t>
   </si>
   <si>
@@ -2003,6 +2000,21 @@
   </si>
   <si>
     <t>Generation_DE GuD Niehl 3 RheinEnergie [MW]</t>
+  </si>
+  <si>
+    <t>Generation_DE Niederaußem G [MW]</t>
+  </si>
+  <si>
+    <t>Generation_DE SWM HKW Sued GuD2 GT61 [MW]</t>
+  </si>
+  <si>
+    <t>Generation_DE GUD C 200 GT 1, GT 2, DT 1 [MW]</t>
+  </si>
+  <si>
+    <t>Generation_DE P [MW]</t>
+  </si>
+  <si>
+    <t>Generation_DE Heizkraftwerk Altbach/Deizisau HKW 2 DT (Solobetrieb) [MW]</t>
   </si>
 </sst>
 </file>
@@ -2104,7 +2116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2115,9 +2127,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -2622,8 +2631,8 @@
   <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2659,13 +2668,13 @@
         <v>168</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>511</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2693,7 +2702,7 @@
       <c r="H2" t="s">
         <v>512</v>
       </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -3119,7 +3128,7 @@
         <v>219</v>
       </c>
       <c r="H18" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -3146,7 +3155,7 @@
         <v>219</v>
       </c>
       <c r="H19" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I19" s="1"/>
     </row>
@@ -3279,7 +3288,7 @@
         <v>224</v>
       </c>
       <c r="H24" t="s">
-        <v>527</v>
+        <v>658</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -3547,7 +3556,7 @@
         <v>229</v>
       </c>
       <c r="H34" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I34" s="1"/>
     </row>
@@ -3657,9 +3666,11 @@
       <c r="H38" t="s">
         <v>543</v>
       </c>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="I38" s="1" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>739</v>
       </c>
@@ -3679,8 +3690,8 @@
       <c r="G39" t="s">
         <v>462</v>
       </c>
-      <c r="H39" s="5" t="s">
-        <v>650</v>
+      <c r="H39" t="s">
+        <v>649</v>
       </c>
       <c r="I39" s="1"/>
     </row>
@@ -3837,7 +3848,7 @@
         <v>187</v>
       </c>
       <c r="G45" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H45" t="s">
         <v>619</v>
@@ -3864,10 +3875,10 @@
         <v>188</v>
       </c>
       <c r="G46" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H46" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="I46" s="1"/>
     </row>
@@ -3894,7 +3905,7 @@
         <v>464</v>
       </c>
       <c r="H47" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I47" s="1"/>
     </row>
@@ -3921,7 +3932,7 @@
         <v>464</v>
       </c>
       <c r="H48" t="s">
-        <v>550</v>
+        <v>656</v>
       </c>
       <c r="I48" s="1"/>
     </row>
@@ -4059,7 +4070,7 @@
         <v>551</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -4349,7 +4360,7 @@
         <v>507</v>
       </c>
       <c r="H64" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I64" s="1"/>
     </row>
@@ -4480,7 +4491,7 @@
         <v>460</v>
       </c>
       <c r="H69" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I69" s="1"/>
     </row>
@@ -4507,7 +4518,7 @@
         <v>460</v>
       </c>
       <c r="H70" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I70" s="1"/>
     </row>
@@ -4534,7 +4545,7 @@
         <v>461</v>
       </c>
       <c r="H71" t="s">
-        <v>567</v>
+        <v>657</v>
       </c>
       <c r="I71" s="1"/>
     </row>
@@ -4561,7 +4572,7 @@
         <v>461</v>
       </c>
       <c r="H72" t="s">
-        <v>567</v>
+        <v>657</v>
       </c>
       <c r="I72" s="1"/>
     </row>
@@ -4615,7 +4626,7 @@
         <v>482</v>
       </c>
       <c r="H74" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I74" s="1"/>
     </row>
@@ -4642,7 +4653,7 @@
         <v>466</v>
       </c>
       <c r="H75" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I75" s="1"/>
     </row>
@@ -4669,7 +4680,7 @@
         <v>466</v>
       </c>
       <c r="H76" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I76" s="1"/>
     </row>
@@ -4694,7 +4705,7 @@
         <v>472</v>
       </c>
       <c r="H77" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I77" s="1"/>
     </row>
@@ -4721,7 +4732,7 @@
         <v>483</v>
       </c>
       <c r="H78" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I78" s="1"/>
     </row>
@@ -4748,7 +4759,7 @@
         <v>487</v>
       </c>
       <c r="H79" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I79" s="1"/>
     </row>
@@ -4775,7 +4786,7 @@
         <v>492</v>
       </c>
       <c r="H80" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I80" s="1"/>
     </row>
@@ -4802,7 +4813,7 @@
         <v>492</v>
       </c>
       <c r="H81" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I81" s="1"/>
     </row>
@@ -4829,7 +4840,7 @@
         <v>495</v>
       </c>
       <c r="H82" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I82" s="1"/>
     </row>
@@ -4856,7 +4867,7 @@
         <v>495</v>
       </c>
       <c r="H83" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I83" s="1"/>
     </row>
@@ -4883,7 +4894,7 @@
         <v>495</v>
       </c>
       <c r="H84" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I84" s="1"/>
     </row>
@@ -4910,7 +4921,7 @@
         <v>495</v>
       </c>
       <c r="H85" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I85" s="1"/>
     </row>
@@ -4937,7 +4948,7 @@
         <v>495</v>
       </c>
       <c r="H86" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I86" s="1"/>
     </row>
@@ -4964,7 +4975,7 @@
         <v>495</v>
       </c>
       <c r="H87" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I87" s="1"/>
     </row>
@@ -4991,7 +5002,7 @@
         <v>473</v>
       </c>
       <c r="H88" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I88" s="1"/>
     </row>
@@ -5018,7 +5029,7 @@
         <v>473</v>
       </c>
       <c r="H89" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I89" s="1"/>
     </row>
@@ -5045,7 +5056,7 @@
         <v>481</v>
       </c>
       <c r="H90" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I90" s="1"/>
     </row>
@@ -5072,7 +5083,7 @@
         <v>501</v>
       </c>
       <c r="H91" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I91" s="1"/>
     </row>
@@ -5099,7 +5110,7 @@
         <v>501</v>
       </c>
       <c r="H92" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I92" s="1"/>
     </row>
@@ -5126,7 +5137,7 @@
         <v>498</v>
       </c>
       <c r="H93" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I93" s="1"/>
     </row>
@@ -5153,7 +5164,7 @@
         <v>477</v>
       </c>
       <c r="H94" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I94" s="1"/>
     </row>
@@ -5180,7 +5191,7 @@
         <v>477</v>
       </c>
       <c r="H95" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I95" s="1"/>
     </row>
@@ -5205,10 +5216,10 @@
         <v>470</v>
       </c>
       <c r="H96" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -5261,7 +5272,7 @@
         <v>469</v>
       </c>
       <c r="H98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I98" s="1"/>
     </row>
@@ -5288,7 +5299,7 @@
         <v>291</v>
       </c>
       <c r="H99" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I99" s="1"/>
     </row>
@@ -5315,7 +5326,7 @@
         <v>291</v>
       </c>
       <c r="H100" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I100" s="1"/>
     </row>
@@ -5342,7 +5353,7 @@
         <v>291</v>
       </c>
       <c r="H101" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="I101" s="1"/>
     </row>
@@ -5369,7 +5380,7 @@
         <v>463</v>
       </c>
       <c r="H102" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I102" s="1"/>
     </row>
@@ -5396,7 +5407,7 @@
         <v>296</v>
       </c>
       <c r="H103" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="I103" s="1"/>
     </row>
@@ -5423,7 +5434,7 @@
         <v>296</v>
       </c>
       <c r="H104" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I104" s="1"/>
     </row>
@@ -5450,7 +5461,7 @@
         <v>252</v>
       </c>
       <c r="H105" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I105" s="1"/>
     </row>
@@ -5477,7 +5488,7 @@
         <v>252</v>
       </c>
       <c r="H106" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I106" s="1"/>
     </row>
@@ -5531,7 +5542,7 @@
         <v>252</v>
       </c>
       <c r="H108" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I108" s="1"/>
     </row>
@@ -5561,7 +5572,7 @@
         <v>527</v>
       </c>
       <c r="I109" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
@@ -5587,10 +5598,10 @@
         <v>252</v>
       </c>
       <c r="H110" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="I110" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
@@ -5616,7 +5627,7 @@
         <v>252</v>
       </c>
       <c r="H111" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I111" s="1"/>
     </row>
@@ -5643,7 +5654,7 @@
         <v>502</v>
       </c>
       <c r="H112" t="s">
-        <v>626</v>
+        <v>655</v>
       </c>
       <c r="I112" s="1"/>
     </row>
@@ -5670,7 +5681,7 @@
         <v>502</v>
       </c>
       <c r="H113" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I113" s="1"/>
     </row>
@@ -5697,7 +5708,7 @@
         <v>502</v>
       </c>
       <c r="H114" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I114" s="1"/>
     </row>
@@ -5724,7 +5735,7 @@
         <v>502</v>
       </c>
       <c r="H115" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I115" s="1"/>
     </row>
@@ -5778,7 +5789,7 @@
         <v>502</v>
       </c>
       <c r="H117" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I117" s="1"/>
     </row>
@@ -5805,7 +5816,7 @@
         <v>502</v>
       </c>
       <c r="H118" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I118" s="1"/>
     </row>
@@ -5832,7 +5843,7 @@
         <v>440</v>
       </c>
       <c r="H119" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I119" s="1"/>
     </row>
@@ -5859,7 +5870,7 @@
         <v>478</v>
       </c>
       <c r="H120" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I120" s="1"/>
     </row>
@@ -5886,7 +5897,7 @@
         <v>478</v>
       </c>
       <c r="H121" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I121" s="1"/>
     </row>
@@ -5913,7 +5924,7 @@
         <v>201</v>
       </c>
       <c r="H122" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I122" s="1"/>
     </row>
@@ -5940,7 +5951,7 @@
         <v>201</v>
       </c>
       <c r="H123" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I123" s="1"/>
     </row>
@@ -5967,7 +5978,7 @@
         <v>201</v>
       </c>
       <c r="H124" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I124" s="1"/>
     </row>
@@ -5994,7 +6005,7 @@
         <v>299</v>
       </c>
       <c r="H125" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I125" s="1"/>
     </row>
@@ -6021,7 +6032,7 @@
         <v>299</v>
       </c>
       <c r="H126" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I126" s="1"/>
     </row>
@@ -6048,7 +6059,7 @@
         <v>263</v>
       </c>
       <c r="H127" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I127" s="1"/>
     </row>
@@ -6075,7 +6086,7 @@
         <v>263</v>
       </c>
       <c r="H128" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I128" s="1"/>
     </row>
@@ -6102,7 +6113,7 @@
         <v>496</v>
       </c>
       <c r="H129" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I129" s="1"/>
     </row>
@@ -6129,13 +6140,13 @@
         <v>496</v>
       </c>
       <c r="H130" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I130" s="1"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
-        <v>1876</v>
+        <v>1786</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>62</v>
@@ -6156,7 +6167,7 @@
         <v>192</v>
       </c>
       <c r="H131" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I131" s="1"/>
     </row>
@@ -6183,7 +6194,7 @@
         <v>192</v>
       </c>
       <c r="H132" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I132" s="1"/>
     </row>
@@ -6210,7 +6221,7 @@
         <v>304</v>
       </c>
       <c r="H133" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I133" s="1"/>
     </row>
@@ -6237,7 +6248,7 @@
         <v>304</v>
       </c>
       <c r="H134" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I134" s="1"/>
     </row>
@@ -6261,10 +6272,10 @@
         <v>10</v>
       </c>
       <c r="G135" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="H135" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I135" s="1"/>
     </row>
@@ -6288,10 +6299,10 @@
         <v>20</v>
       </c>
       <c r="G136" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="H136" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I136" s="1"/>
     </row>
@@ -6318,7 +6329,7 @@
         <v>505</v>
       </c>
       <c r="H137" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I137" s="1"/>
     </row>
@@ -6345,7 +6356,7 @@
         <v>468</v>
       </c>
       <c r="H138" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I138" s="1"/>
     </row>
@@ -6372,7 +6383,7 @@
         <v>468</v>
       </c>
       <c r="H139" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I139" s="1"/>
     </row>
@@ -6399,7 +6410,7 @@
         <v>305</v>
       </c>
       <c r="H140" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I140" s="1"/>
     </row>
@@ -6426,7 +6437,7 @@
         <v>305</v>
       </c>
       <c r="H141" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I141" s="1"/>
     </row>
@@ -6453,7 +6464,7 @@
         <v>273</v>
       </c>
       <c r="H142" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I142" s="1"/>
     </row>
@@ -6480,7 +6491,7 @@
         <v>275</v>
       </c>
       <c r="H143" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I143" s="1"/>
     </row>
@@ -6507,7 +6518,7 @@
         <v>275</v>
       </c>
       <c r="H144" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I144" s="1"/>
     </row>
@@ -6534,7 +6545,7 @@
         <v>275</v>
       </c>
       <c r="H145" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I145" s="1"/>
     </row>
@@ -6561,7 +6572,7 @@
         <v>275</v>
       </c>
       <c r="H146" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I146" s="1"/>
     </row>
@@ -6588,7 +6599,7 @@
         <v>275</v>
       </c>
       <c r="H147" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I147" s="1"/>
     </row>
@@ -6615,7 +6626,7 @@
         <v>275</v>
       </c>
       <c r="H148" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I148" s="1"/>
     </row>
@@ -6642,7 +6653,7 @@
         <v>279</v>
       </c>
       <c r="H149" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I149" s="1"/>
     </row>
@@ -6669,7 +6680,7 @@
         <v>279</v>
       </c>
       <c r="H150" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I150" s="1"/>
     </row>
@@ -6696,7 +6707,7 @@
         <v>196</v>
       </c>
       <c r="H151" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I151" s="1"/>
     </row>
@@ -6720,12 +6731,12 @@
         <v>5</v>
       </c>
       <c r="G152" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H152" t="s">
-        <v>624</v>
-      </c>
-      <c r="I152" s="7"/>
+        <v>623</v>
+      </c>
+      <c r="I152" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F152">

</xml_diff>

<commit_message>
Updated to 2023, Corrected Processing Step
</commit_message>
<xml_diff>
--- a/input/blocks.xlsx
+++ b/input/blocks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\Documents\09_Job\HiWi\02_Projekte\smard-data-processing\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A718BA85-5541-4692-B036-BA0FAD5079BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96937AB4-5DE6-4E84-A703-934AFA40025D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3864E39-C3D2-F749-9175-08B59E08C58D}"/>
   </bookViews>
@@ -2064,7 +2064,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2098,37 +2098,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2140,31 +2114,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -2323,22 +2277,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{849F333F-5B1A-4F37-83E1-1E8DD224AF6E}" name="Tabelle1" displayName="Tabelle1" ref="A1:J152" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{849F333F-5B1A-4F37-83E1-1E8DD224AF6E}" name="Tabelle1" displayName="Tabelle1" ref="A1:J152" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:J152" xr:uid="{849F333F-5B1A-4F37-83E1-1E8DD224AF6E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J152">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I152">
     <sortCondition descending="1" ref="G1:G152"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4F422979-A991-4E34-A517-EFD215C88D16}" name="ETS-ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{5F0E830E-86FF-4A7B-99B2-48E60507FF39}" name="EIC" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{6F4402A2-BFDB-47AC-A995-59F52E01E1AB}" name="Name BNA" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{50C60119-F5E5-45EF-BD10-1589670828EB}" name="City" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{82C3D041-2B42-4975-A236-8BD3A731F36B}" name="Plant name" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{31D64339-73C5-4BE1-A253-730B40AB0E01}" name="Block name" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{4F422979-A991-4E34-A517-EFD215C88D16}" name="ETS-ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{5F0E830E-86FF-4A7B-99B2-48E60507FF39}" name="EIC" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{6F4402A2-BFDB-47AC-A995-59F52E01E1AB}" name="Name BNA" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{50C60119-F5E5-45EF-BD10-1589670828EB}" name="City" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{82C3D041-2B42-4975-A236-8BD3A731F36B}" name="Plant name" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{31D64339-73C5-4BE1-A253-730B40AB0E01}" name="Block name" dataDxfId="0"/>
     <tableColumn id="18" xr3:uid="{259FB2C6-E6F8-4F55-81FC-D301978B55C3}" name="Filename"/>
     <tableColumn id="19" xr3:uid="{9E5B4CF5-DBA3-4D57-9058-4118952E7026}" name="Column_Block_Smard"/>
     <tableColumn id="3" xr3:uid="{2029C437-FAEA-4156-ADC3-30DEFB43CC54}" name="Column_Block_Smard_2"/>
-    <tableColumn id="14" xr3:uid="{3BAD55D8-7D72-4AF3-943E-CF0B9F327441}" name="Column_Block_Smard_Alternative" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{C2437449-8420-4DFE-8E6B-D16EE67AE778}" name="Column_Block_Smard_Alternative"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2644,13 +2598,13 @@
   <dimension ref="A1:J152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="1" max="1" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.09765625" customWidth="1"/>
@@ -2659,7 +2613,7 @@
     <col min="7" max="7" width="39.8984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="87.59765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="64.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -2719,7 +2673,6 @@
       <c r="H2" t="s">
         <v>644</v>
       </c>
-      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -2747,7 +2700,6 @@
         <v>597</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -2774,7 +2726,6 @@
       <c r="H4" t="s">
         <v>596</v>
       </c>
-      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -2801,7 +2752,6 @@
       <c r="H5" t="s">
         <v>596</v>
       </c>
-      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -2828,7 +2778,6 @@
       <c r="H6" t="s">
         <v>643</v>
       </c>
-      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -2855,7 +2804,6 @@
       <c r="H7" t="s">
         <v>642</v>
       </c>
-      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -2882,7 +2830,6 @@
       <c r="H8" t="s">
         <v>639</v>
       </c>
-      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -2909,7 +2856,6 @@
       <c r="H9" t="s">
         <v>641</v>
       </c>
-      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -2936,7 +2882,6 @@
       <c r="H10" t="s">
         <v>640</v>
       </c>
-      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -2963,7 +2908,6 @@
       <c r="H11" t="s">
         <v>613</v>
       </c>
-      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -2990,7 +2934,6 @@
       <c r="H12" t="s">
         <v>612</v>
       </c>
-      <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -3017,7 +2960,6 @@
       <c r="H13" t="s">
         <v>611</v>
       </c>
-      <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -3044,7 +2986,6 @@
       <c r="H14" t="s">
         <v>638</v>
       </c>
-      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -3071,7 +3012,6 @@
       <c r="H15" t="s">
         <v>637</v>
       </c>
-      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -3098,9 +3038,8 @@
       <c r="H16" t="s">
         <v>610</v>
       </c>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2195</v>
       </c>
@@ -3125,9 +3064,8 @@
       <c r="H17" t="s">
         <v>614</v>
       </c>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2195</v>
       </c>
@@ -3152,9 +3090,8 @@
       <c r="H18" t="s">
         <v>615</v>
       </c>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>951</v>
       </c>
@@ -3179,9 +3116,8 @@
       <c r="H19" t="s">
         <v>608</v>
       </c>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>951</v>
       </c>
@@ -3206,9 +3142,8 @@
       <c r="H20" t="s">
         <v>609</v>
       </c>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1876</v>
       </c>
@@ -3233,9 +3168,8 @@
       <c r="H21" t="s">
         <v>606</v>
       </c>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1876</v>
       </c>
@@ -3260,9 +3194,8 @@
       <c r="H22" t="s">
         <v>607</v>
       </c>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1459</v>
       </c>
@@ -3287,9 +3220,8 @@
       <c r="H23" t="s">
         <v>635</v>
       </c>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1459</v>
       </c>
@@ -3314,9 +3246,8 @@
       <c r="H24" t="s">
         <v>636</v>
       </c>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1205</v>
       </c>
@@ -3341,9 +3272,8 @@
       <c r="H25" t="s">
         <v>633</v>
       </c>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1205</v>
       </c>
@@ -3368,9 +3298,8 @@
       <c r="H26" t="s">
         <v>634</v>
       </c>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1376</v>
       </c>
@@ -3395,9 +3324,8 @@
       <c r="H27" t="s">
         <v>598</v>
       </c>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1376</v>
       </c>
@@ -3422,9 +3350,8 @@
       <c r="H28" t="s">
         <v>605</v>
       </c>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1457</v>
       </c>
@@ -3449,9 +3376,8 @@
       <c r="H29" t="s">
         <v>602</v>
       </c>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1457</v>
       </c>
@@ -3476,9 +3402,8 @@
       <c r="H30" t="s">
         <v>603</v>
       </c>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>1457</v>
       </c>
@@ -3503,9 +3428,8 @@
       <c r="H31" t="s">
         <v>604</v>
       </c>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>1179</v>
       </c>
@@ -3530,7 +3454,6 @@
       <c r="H32" t="s">
         <v>600</v>
       </c>
-      <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
@@ -3557,7 +3480,6 @@
       <c r="H33" t="s">
         <v>601</v>
       </c>
-      <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
@@ -3584,7 +3506,6 @@
       <c r="H34" t="s">
         <v>599</v>
       </c>
-      <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
@@ -3611,7 +3532,6 @@
       <c r="H35" t="s">
         <v>597</v>
       </c>
-      <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
@@ -3638,7 +3558,6 @@
       <c r="H36" t="s">
         <v>518</v>
       </c>
-      <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
@@ -3665,7 +3584,6 @@
       <c r="H37" t="s">
         <v>630</v>
       </c>
-      <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
@@ -3692,7 +3610,6 @@
       <c r="H38" t="s">
         <v>624</v>
       </c>
-      <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
@@ -3719,7 +3636,6 @@
       <c r="H39" t="s">
         <v>654</v>
       </c>
-      <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
@@ -3746,7 +3662,6 @@
       <c r="H40" t="s">
         <v>631</v>
       </c>
-      <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
@@ -3773,7 +3688,6 @@
       <c r="H41" t="s">
         <v>632</v>
       </c>
-      <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
@@ -3800,7 +3714,6 @@
       <c r="H42" t="s">
         <v>598</v>
       </c>
-      <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
@@ -3827,7 +3740,6 @@
       <c r="H43" t="s">
         <v>558</v>
       </c>
-      <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
@@ -3854,7 +3766,6 @@
       <c r="H44" t="s">
         <v>627</v>
       </c>
-      <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
@@ -3881,7 +3792,6 @@
       <c r="H45" t="s">
         <v>628</v>
       </c>
-      <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
@@ -3908,7 +3818,6 @@
       <c r="H46" t="s">
         <v>629</v>
       </c>
-      <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
@@ -3993,7 +3902,6 @@
       <c r="H49" t="s">
         <v>593</v>
       </c>
-      <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
@@ -4020,7 +3928,6 @@
       <c r="H50" t="s">
         <v>594</v>
       </c>
-      <c r="J50" s="1"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
@@ -4047,7 +3954,6 @@
       <c r="H51" t="s">
         <v>626</v>
       </c>
-      <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
@@ -4074,7 +3980,6 @@
       <c r="H52" t="s">
         <v>592</v>
       </c>
-      <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
@@ -4101,7 +4006,6 @@
       <c r="H53" t="s">
         <v>590</v>
       </c>
-      <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
@@ -4128,7 +4032,6 @@
       <c r="H54" t="s">
         <v>591</v>
       </c>
-      <c r="J54" s="1"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
@@ -4155,7 +4058,6 @@
       <c r="H55" t="s">
         <v>588</v>
       </c>
-      <c r="J55" s="1"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
@@ -4182,7 +4084,6 @@
       <c r="H56" t="s">
         <v>558</v>
       </c>
-      <c r="J56" s="1"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
@@ -4236,7 +4137,6 @@
       <c r="H58" t="s">
         <v>586</v>
       </c>
-      <c r="J58" s="1"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
@@ -4263,7 +4163,6 @@
       <c r="H59" t="s">
         <v>585</v>
       </c>
-      <c r="J59" s="1"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
@@ -4290,7 +4189,6 @@
       <c r="H60" t="s">
         <v>625</v>
       </c>
-      <c r="J60" s="1"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
@@ -4317,7 +4215,6 @@
       <c r="H61" t="s">
         <v>583</v>
       </c>
-      <c r="J61" s="1"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
@@ -4344,7 +4241,6 @@
       <c r="H62" t="s">
         <v>584</v>
       </c>
-      <c r="J62" s="1"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
@@ -4371,7 +4267,6 @@
       <c r="H63" t="s">
         <v>582</v>
       </c>
-      <c r="J63" s="1"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
@@ -4398,9 +4293,8 @@
       <c r="H64" t="s">
         <v>581</v>
       </c>
-      <c r="J64" s="1"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>1064</v>
       </c>
@@ -4425,9 +4319,8 @@
       <c r="H65" t="s">
         <v>580</v>
       </c>
-      <c r="J65" s="1"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>1456</v>
       </c>
@@ -4452,9 +4345,8 @@
       <c r="H66" t="s">
         <v>574</v>
       </c>
-      <c r="J66" s="1"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>1456</v>
       </c>
@@ -4479,9 +4371,8 @@
       <c r="H67" t="s">
         <v>579</v>
       </c>
-      <c r="J67" s="1"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>1456</v>
       </c>
@@ -4506,9 +4397,8 @@
       <c r="H68" t="s">
         <v>578</v>
       </c>
-      <c r="J68" s="1"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>1456</v>
       </c>
@@ -4533,9 +4423,8 @@
       <c r="H69" t="s">
         <v>577</v>
       </c>
-      <c r="J69" s="1"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>1456</v>
       </c>
@@ -4560,9 +4449,8 @@
       <c r="H70" t="s">
         <v>576</v>
       </c>
-      <c r="J70" s="1"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>1456</v>
       </c>
@@ -4587,9 +4475,8 @@
       <c r="H71" t="s">
         <v>575</v>
       </c>
-      <c r="J71" s="1"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>1447</v>
       </c>
@@ -4614,9 +4501,8 @@
       <c r="H72" t="s">
         <v>572</v>
       </c>
-      <c r="J72" s="1"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>1447</v>
       </c>
@@ -4641,9 +4527,8 @@
       <c r="H73" t="s">
         <v>573</v>
       </c>
-      <c r="J73" s="1"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>1312</v>
       </c>
@@ -4668,9 +4553,8 @@
       <c r="H74" t="s">
         <v>571</v>
       </c>
-      <c r="J74" s="1"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>1253</v>
       </c>
@@ -4695,9 +4579,8 @@
       <c r="H75" t="s">
         <v>570</v>
       </c>
-      <c r="J75" s="1"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>999</v>
       </c>
@@ -4720,9 +4603,8 @@
       <c r="H76" t="s">
         <v>569</v>
       </c>
-      <c r="J76" s="1"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>839</v>
       </c>
@@ -4747,9 +4629,8 @@
       <c r="H77" t="s">
         <v>568</v>
       </c>
-      <c r="J77" s="1"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>838</v>
       </c>
@@ -4774,9 +4655,8 @@
       <c r="H78" t="s">
         <v>567</v>
       </c>
-      <c r="J78" s="1"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>1238</v>
       </c>
@@ -4801,9 +4681,8 @@
       <c r="H79" t="s">
         <v>566</v>
       </c>
-      <c r="J79" s="1"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>852</v>
       </c>
@@ -4828,9 +4707,8 @@
       <c r="H80" t="s">
         <v>565</v>
       </c>
-      <c r="J80" s="1"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>1484</v>
       </c>
@@ -4855,9 +4733,8 @@
       <c r="H81" t="s">
         <v>656</v>
       </c>
-      <c r="J81" s="1"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>1484</v>
       </c>
@@ -4882,9 +4759,8 @@
       <c r="H82" t="s">
         <v>656</v>
       </c>
-      <c r="J82" s="1"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>662</v>
       </c>
@@ -4909,9 +4785,8 @@
       <c r="H83" t="s">
         <v>616</v>
       </c>
-      <c r="J83" s="1"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>662</v>
       </c>
@@ -4936,9 +4811,8 @@
       <c r="H84" t="s">
         <v>663</v>
       </c>
-      <c r="J84" s="1"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>1309</v>
       </c>
@@ -4961,9 +4835,8 @@
       <c r="H85" t="s">
         <v>564</v>
       </c>
-      <c r="J85" s="1"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>202777</v>
       </c>
@@ -4988,9 +4861,8 @@
       <c r="H86" t="s">
         <v>562</v>
       </c>
-      <c r="J86" s="1"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>1786</v>
       </c>
@@ -5015,9 +4887,8 @@
       <c r="H87" t="s">
         <v>563</v>
       </c>
-      <c r="J87" s="1"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>1170</v>
       </c>
@@ -5040,9 +4911,8 @@
       <c r="H88" t="s">
         <v>561</v>
       </c>
-      <c r="J88" s="1"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>210483</v>
       </c>
@@ -5065,9 +4935,8 @@
       <c r="H89" t="s">
         <v>589</v>
       </c>
-      <c r="J89" s="1"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>19</v>
       </c>
@@ -5092,9 +4961,8 @@
       <c r="H90" t="s">
         <v>559</v>
       </c>
-      <c r="J90" s="1"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>19</v>
       </c>
@@ -5119,9 +4987,8 @@
       <c r="H91" t="s">
         <v>560</v>
       </c>
-      <c r="J91" s="1"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>1480</v>
       </c>
@@ -5146,9 +5013,8 @@
       <c r="H92" t="s">
         <v>558</v>
       </c>
-      <c r="J92" s="1"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>995</v>
       </c>
@@ -5171,9 +5037,8 @@
       <c r="H93" t="s">
         <v>557</v>
       </c>
-      <c r="J93" s="1"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>1486</v>
       </c>
@@ -5198,9 +5063,8 @@
       <c r="H94" t="s">
         <v>555</v>
       </c>
-      <c r="J94" s="1"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>1486</v>
       </c>
@@ -5225,9 +5089,8 @@
       <c r="H95" t="s">
         <v>556</v>
       </c>
-      <c r="J95" s="1"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>1291</v>
       </c>
@@ -5250,7 +5113,6 @@
       <c r="H96" t="s">
         <v>554</v>
       </c>
-      <c r="J96" s="1"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
@@ -5277,7 +5139,6 @@
       <c r="H97" t="s">
         <v>552</v>
       </c>
-      <c r="J97" s="1"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
@@ -5304,7 +5165,6 @@
       <c r="H98" t="s">
         <v>553</v>
       </c>
-      <c r="J98" s="1"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
@@ -5334,7 +5194,6 @@
       <c r="I99" t="s">
         <v>662</v>
       </c>
-      <c r="J99" s="1"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
@@ -5361,7 +5220,6 @@
       <c r="H100" t="s">
         <v>525</v>
       </c>
-      <c r="J100" s="1"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
@@ -5388,7 +5246,6 @@
       <c r="H101" t="s">
         <v>525</v>
       </c>
-      <c r="J101" s="1"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
@@ -5444,7 +5301,6 @@
       <c r="H103" t="s">
         <v>548</v>
       </c>
-      <c r="J103" s="1"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
@@ -5471,7 +5327,6 @@
       <c r="H104" t="s">
         <v>645</v>
       </c>
-      <c r="J104" s="1"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
@@ -5498,7 +5353,6 @@
       <c r="H105" t="s">
         <v>655</v>
       </c>
-      <c r="J105" s="1"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
@@ -5525,7 +5379,6 @@
       <c r="H106" t="s">
         <v>549</v>
       </c>
-      <c r="J106" s="1"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
@@ -5552,7 +5405,6 @@
       <c r="H107" t="s">
         <v>618</v>
       </c>
-      <c r="J107" s="1"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
@@ -5579,7 +5431,6 @@
       <c r="H108" t="s">
         <v>617</v>
       </c>
-      <c r="J108" s="1"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
@@ -5656,7 +5507,6 @@
       <c r="H111" t="s">
         <v>545</v>
       </c>
-      <c r="J111" s="1"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
@@ -5683,9 +5533,8 @@
       <c r="H112" t="s">
         <v>547</v>
       </c>
-      <c r="J112" s="1"/>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>1452</v>
       </c>
@@ -5710,9 +5559,8 @@
       <c r="H113" t="s">
         <v>544</v>
       </c>
-      <c r="J113" s="1"/>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>739</v>
       </c>
@@ -5735,9 +5583,8 @@
       <c r="H114" t="s">
         <v>648</v>
       </c>
-      <c r="J114" s="1"/>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>1450</v>
       </c>
@@ -5762,9 +5609,8 @@
       <c r="H115" t="s">
         <v>543</v>
       </c>
-      <c r="J115" s="1"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>1450</v>
       </c>
@@ -5789,9 +5635,8 @@
       <c r="H116" t="s">
         <v>658</v>
       </c>
-      <c r="J116" s="1"/>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>1387</v>
       </c>
@@ -5816,9 +5661,8 @@
       <c r="H117" t="s">
         <v>538</v>
       </c>
-      <c r="J117" s="1"/>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>1387</v>
       </c>
@@ -5843,9 +5687,8 @@
       <c r="H118" t="s">
         <v>539</v>
       </c>
-      <c r="J118" s="1"/>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>1481</v>
       </c>
@@ -5870,9 +5713,8 @@
       <c r="H119" t="s">
         <v>531</v>
       </c>
-      <c r="J119" s="1"/>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>1481</v>
       </c>
@@ -5897,9 +5739,8 @@
       <c r="H120" t="s">
         <v>532</v>
       </c>
-      <c r="J120" s="1"/>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>1481</v>
       </c>
@@ -5927,9 +5768,8 @@
       <c r="I121" t="s">
         <v>659</v>
       </c>
-      <c r="J121" s="1"/>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>1481</v>
       </c>
@@ -5954,9 +5794,8 @@
       <c r="H122" t="s">
         <v>529</v>
       </c>
-      <c r="J122" s="1"/>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>1481</v>
       </c>
@@ -5981,9 +5820,8 @@
       <c r="H123" t="s">
         <v>623</v>
       </c>
-      <c r="J123" s="1"/>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>1210</v>
       </c>
@@ -6006,9 +5844,8 @@
       <c r="H124" t="s">
         <v>530</v>
       </c>
-      <c r="J124" s="1"/>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>1207</v>
       </c>
@@ -6033,9 +5870,8 @@
       <c r="H125" t="s">
         <v>536</v>
       </c>
-      <c r="J125" s="1"/>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>4148</v>
       </c>
@@ -6060,9 +5896,8 @@
       <c r="H126" t="s">
         <v>537</v>
       </c>
-      <c r="J126" s="1"/>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>1207</v>
       </c>
@@ -6087,9 +5922,8 @@
       <c r="H127" t="s">
         <v>542</v>
       </c>
-      <c r="J127" s="1"/>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>1605</v>
       </c>
@@ -6114,9 +5948,8 @@
       <c r="H128" t="s">
         <v>657</v>
       </c>
-      <c r="J128" s="1"/>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>1605</v>
       </c>
@@ -6141,9 +5974,8 @@
       <c r="H129" t="s">
         <v>528</v>
       </c>
-      <c r="J129" s="1"/>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>1446</v>
       </c>
@@ -6168,9 +6000,8 @@
       <c r="H130" t="s">
         <v>524</v>
       </c>
-      <c r="J130" s="1"/>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>1446</v>
       </c>
@@ -6195,9 +6026,8 @@
       <c r="H131" t="s">
         <v>526</v>
       </c>
-      <c r="J131" s="1"/>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>969</v>
       </c>
@@ -6220,9 +6050,8 @@
       <c r="H132" t="s">
         <v>541</v>
       </c>
-      <c r="J132" s="1"/>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>1479</v>
       </c>
@@ -6247,9 +6076,8 @@
       <c r="H133" t="s">
         <v>619</v>
       </c>
-      <c r="J133" s="1"/>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>1479</v>
       </c>
@@ -6274,9 +6102,8 @@
       <c r="H134" t="s">
         <v>620</v>
       </c>
-      <c r="J134" s="1"/>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>1479</v>
       </c>
@@ -6301,9 +6128,8 @@
       <c r="H135" t="s">
         <v>518</v>
       </c>
-      <c r="J135" s="1"/>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>1415</v>
       </c>
@@ -6328,9 +6154,8 @@
       <c r="H136" t="s">
         <v>523</v>
       </c>
-      <c r="J136" s="1"/>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>1174</v>
       </c>
@@ -6355,9 +6180,8 @@
       <c r="H137" t="s">
         <v>540</v>
       </c>
-      <c r="J137" s="1"/>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>1411</v>
       </c>
@@ -6382,9 +6206,8 @@
       <c r="H138" t="s">
         <v>521</v>
       </c>
-      <c r="J138" s="1"/>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>1850</v>
       </c>
@@ -6409,9 +6232,8 @@
       <c r="H139" t="s">
         <v>522</v>
       </c>
-      <c r="J139" s="1"/>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>1485</v>
       </c>
@@ -6436,9 +6258,8 @@
       <c r="H140" t="s">
         <v>525</v>
       </c>
-      <c r="J140" s="1"/>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>208968</v>
       </c>
@@ -6463,9 +6284,8 @@
       <c r="H141" t="s">
         <v>520</v>
       </c>
-      <c r="J141" s="1"/>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>1409</v>
       </c>
@@ -6490,9 +6310,8 @@
       <c r="H142" t="s">
         <v>517</v>
       </c>
-      <c r="J142" s="1"/>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>1419</v>
       </c>
@@ -6515,9 +6334,8 @@
       <c r="H143" t="s">
         <v>518</v>
       </c>
-      <c r="J143" s="1"/>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>795</v>
       </c>
@@ -6543,9 +6361,8 @@
       <c r="I144" t="s">
         <v>661</v>
       </c>
-      <c r="J144" s="1"/>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>1460</v>
       </c>
@@ -6570,9 +6387,8 @@
       <c r="H145" t="s">
         <v>534</v>
       </c>
-      <c r="J145" s="1"/>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>1460</v>
       </c>
@@ -6597,9 +6413,8 @@
       <c r="H146" t="s">
         <v>535</v>
       </c>
-      <c r="J146" s="1"/>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>1453</v>
       </c>
@@ -6624,9 +6439,8 @@
       <c r="H147" t="s">
         <v>513</v>
       </c>
-      <c r="J147" s="1"/>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>1453</v>
       </c>
@@ -6651,9 +6465,8 @@
       <c r="H148" t="s">
         <v>514</v>
       </c>
-      <c r="J148" s="1"/>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>1454</v>
       </c>
@@ -6678,9 +6491,8 @@
       <c r="H149" t="s">
         <v>515</v>
       </c>
-      <c r="J149" s="1"/>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>1454</v>
       </c>
@@ -6705,9 +6517,8 @@
       <c r="H150" t="s">
         <v>516</v>
       </c>
-      <c r="J150" s="1"/>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>1399</v>
       </c>
@@ -6732,9 +6543,8 @@
       <c r="H151" t="s">
         <v>512</v>
       </c>
-      <c r="J151" s="1"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>1194</v>
       </c>
@@ -6759,7 +6569,6 @@
       <c r="H152" t="s">
         <v>622</v>
       </c>
-      <c r="J152" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F152">

</xml_diff>